<commit_message>
cambios de caso de prueba 7 y 8
</commit_message>
<xml_diff>
--- a/Casos de prueba/TC-6.xlsx
+++ b/Casos de prueba/TC-6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\TestingAplicaciones-HDP-TPO\Casos de prueba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A033F91D-9AFC-439D-8FA8-86E4063C9923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB6ED20-4AA3-49EA-AD3A-DF7FA01B7879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{B9FDB8B2-3DAD-4091-95BA-CDD5EE4AD8A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -107,15 +107,6 @@
     <t>Regression 4</t>
   </si>
   <si>
-    <t>Tester: Sam Peters</t>
-  </si>
-  <si>
-    <t>Tester: Jane Williams</t>
-  </si>
-  <si>
-    <t>Tester:</t>
-  </si>
-  <si>
     <t>Step #</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
     <t>Credential can be entered</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>Defects Created</t>
   </si>
   <si>
@@ -213,13 +201,28 @@
   </si>
   <si>
     <t xml:space="preserve">18 &gt;= user </t>
+  </si>
+  <si>
+    <t>Tester: Camila Sturlesi</t>
+  </si>
+  <si>
+    <t>Tester: Martina Degui</t>
+  </si>
+  <si>
+    <t>Tester: Sebastian Deina</t>
+  </si>
+  <si>
+    <t>Tester:  Lucas Argerich</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,14 +286,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -342,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -626,6 +621,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -634,7 +642,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -684,37 +692,34 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -762,15 +767,66 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -783,62 +839,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1160,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753BCD2C-D1E9-43CA-8B7A-EB7A177E68D9}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,15 +1183,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="57"/>
+      <c r="D1" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1199,23 +1201,23 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="45"/>
+    </row>
+    <row r="3" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="58"/>
-    </row>
-    <row r="3" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="29" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>6.1</v>
       </c>
       <c r="F3" s="6"/>
@@ -1240,7 +1242,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="11" t="s">
@@ -1260,11 +1262,11 @@
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="36">
+      <c r="D6" s="35">
         <v>1</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>39</v>
+      <c r="E6" s="34" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1274,11 +1276,11 @@
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="35">
         <v>2</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>40</v>
+      <c r="E7" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
@@ -1288,10 +1290,10 @@
       <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="35">
         <v>3</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1300,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="36">
+        <v>54</v>
+      </c>
+      <c r="D9" s="35">
         <v>4</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>41</v>
+      <c r="E9" s="34" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1314,11 +1316,11 @@
         <v>3</v>
       </c>
       <c r="B10" s="14"/>
-      <c r="D10" s="36">
+      <c r="D10" s="35">
         <v>5</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>51</v>
+      <c r="E10" s="34" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1326,92 +1328,92 @@
         <v>4</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="D11" s="36">
+      <c r="D11" s="35">
         <v>6</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="34" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="36">
+      <c r="D12" s="35">
         <v>7</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>42</v>
+      <c r="E12" s="34" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="36">
+      <c r="D13" s="35">
         <v>8</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>43</v>
+      <c r="E13" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="36">
+      <c r="D14" s="35">
         <v>9</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>44</v>
+      <c r="E14" s="34" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="36">
+      <c r="D15" s="35">
         <v>10</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>56</v>
+      <c r="E15" s="34" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="63"/>
+      <c r="B22" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="50"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
     </row>
     <row r="24" spans="1:14" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="67" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="68"/>
+      <c r="B24" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="55"/>
       <c r="D24" s="16" t="s">
         <v>17</v>
       </c>
@@ -1419,143 +1421,147 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+    <row r="25" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="53" t="s">
+      <c r="G25" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="55"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="57"/>
     </row>
     <row r="26" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E26" s="22"/>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="51"/>
-      <c r="I26" s="50" t="s">
+      <c r="H26" s="57"/>
+      <c r="I26" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="51"/>
-      <c r="K26" s="50" t="s">
+      <c r="J26" s="57"/>
+      <c r="K26" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="L26" s="51"/>
-      <c r="M26" s="50" t="s">
+      <c r="L26" s="57"/>
+      <c r="M26" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="N26" s="51"/>
+      <c r="N26" s="57"/>
     </row>
     <row r="27" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
         <v>1</v>
       </c>
-      <c r="B27" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="45"/>
-      <c r="G27" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="51"/>
-      <c r="I27" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="N27" s="51"/>
+      <c r="B27" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="59"/>
+      <c r="G27" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="57"/>
+      <c r="I27" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="60"/>
+      <c r="K27" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="L27" s="57"/>
+      <c r="M27" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="N27" s="57"/>
     </row>
     <row r="28" spans="1:14" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24">
         <v>2</v>
       </c>
-      <c r="B28" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="45"/>
+      <c r="B28" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="59"/>
       <c r="G28" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L28" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M28" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N28" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
         <v>3</v>
       </c>
-      <c r="B29" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="G29" s="25" t="s">
-        <v>33</v>
+      <c r="B29" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="59"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="59"/>
+      <c r="G29" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="H29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="25" t="s">
-        <v>33</v>
+      <c r="I29" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K29" s="25" t="s">
-        <v>33</v>
+      <c r="K29" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="L29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="25"/>
+      <c r="M29" s="42" t="s">
+        <v>30</v>
+      </c>
       <c r="N29" s="15" t="s">
         <v>11</v>
       </c>
@@ -1564,31 +1570,33 @@
       <c r="A30" s="24">
         <v>4</v>
       </c>
-      <c r="B30" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
-      <c r="G30" s="25" t="s">
-        <v>33</v>
+      <c r="B30" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="61"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+      <c r="G30" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="H30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="25" t="s">
-        <v>33</v>
+      <c r="I30" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="J30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K30" s="25" t="s">
-        <v>33</v>
+      <c r="K30" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="L30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="25"/>
+      <c r="M30" s="42" t="s">
+        <v>30</v>
+      </c>
       <c r="N30" s="15" t="s">
         <v>11</v>
       </c>
@@ -1597,34 +1605,36 @@
       <c r="A31" s="24">
         <v>5</v>
       </c>
-      <c r="B31" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="45"/>
-      <c r="G31" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="40" t="s">
+      <c r="B31" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="61"/>
+      <c r="D31" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="59"/>
+      <c r="G31" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="K31" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="L31" s="40" t="s">
+      <c r="I31" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="39"/>
-      <c r="N31" s="40" t="s">
+      <c r="M31" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="N31" s="39" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1632,124 +1642,129 @@
       <c r="A32" s="24">
         <v>6</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="48"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="64"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G36" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="N36" s="26"/>
+      <c r="G36" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" s="25"/>
     </row>
     <row r="37" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="26"/>
+      <c r="N37" s="26"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B22:E23"/>
-    <mergeCell ref="B24:C24"/>
+  <mergeCells count="27">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="K26:L26"/>
@@ -1757,19 +1772,15 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:L27"/>
     <mergeCell ref="M27:N27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B22:E23"/>
+    <mergeCell ref="B24:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="120" verticalDpi="72" r:id="rId1"/>

</xml_diff>